<commit_message>
Update key commentary and summary files for CCAR 2025 and 2026 Proposed
Refined key commentary and summary markdown files to remove computed markers for economic indicators, enhancing clarity. Updated JSON configurations to reflect changes in naming conventions for US Real GDP and US Unemployment. Adjusted data processing scripts to support these updates, ensuring consistent formatting across all outputs.
</commit_message>
<xml_diff>
--- a/artifacts/2025/table_vs_avg_gfc.xlsx
+++ b/artifacts/2025/table_vs_avg_gfc.xlsx
@@ -586,7 +586,7 @@
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>Real GDP</t>
+          <t>US Real GDP</t>
         </is>
       </c>
       <c r="C2" s="6" t="inlineStr">
@@ -611,7 +611,7 @@
       <c r="A3" s="9" t="n"/>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>Unemployment</t>
+          <t>US Unemployment</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
@@ -1008,12 +1008,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A15:A17"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance run_all.py and update Excel export scripts for improved clarity and functionality
Added a new script for timeline generation to the execution sequence in run_all.py. Updated argument parsing to change the scenario identifier to a year identifier for better clarity. Modified Excel export scripts to change header colors for improved visual distinction. Adjusted row heights in the historical comparison export to enhance readability. Updated JSON configurations to remove redundant symbols for economic indicators.
</commit_message>
<xml_diff>
--- a/artifacts/2025/table_vs_avg_gfc.xlsx
+++ b/artifacts/2025/table_vs_avg_gfc.xlsx
@@ -50,8 +50,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="001F2937"/>
-        <bgColor rgb="001F2937"/>
+        <fgColor rgb="000000FF"/>
+        <bgColor rgb="000000FF"/>
       </patternFill>
     </fill>
     <fill>

</xml_diff>